<commit_message>
Support any currency in comment (XXX X.XX/ SHR) and always round share count to integer
</commit_message>
<xml_diff>
--- a/data/demo_XTB_broker_statement.xlsx
+++ b/data/demo_XTB_broker_statement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wojci\OneDrive\Dokumenty\GitHub\xtb-dividend-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2A22BB-DBBC-4239-B7CE-7D8912E957B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FFD52B-876F-4ADA-B7EC-6368539DE120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="3" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
+    <workbookView xWindow="57480" yWindow="6735" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
   </bookViews>
   <sheets>
     <sheet name="CLOSED POSITION HISTORY" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="116">
   <si>
     <r>
       <rPr>
@@ -400,9 +400,6 @@
     <t>SBUX.US USD 0.5700/ SHR</t>
   </si>
   <si>
-    <t>SBUX.US USD WHT 30%</t>
-  </si>
-  <si>
     <t>SBUX.US USD WHT 15%</t>
   </si>
   <si>
@@ -452,6 +449,42 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>NVO.US USD 0.5848/ SHR</t>
+  </si>
+  <si>
+    <t>NVO.US</t>
+  </si>
+  <si>
+    <t>NVO.US USD WHT 27%</t>
+  </si>
+  <si>
+    <t>NOVOB.DK DKK 3.7500/ SHR</t>
+  </si>
+  <si>
+    <t>NOVOB.DK</t>
+  </si>
+  <si>
+    <t>NOVOB.DK DKK WHT 27%</t>
+  </si>
+  <si>
+    <t>ASB.PL USD 0.3000/ SHR</t>
+  </si>
+  <si>
+    <t>ASB.PL</t>
+  </si>
+  <si>
+    <t>XTB.PL PLN 5.4500/ SHR</t>
+  </si>
+  <si>
+    <t>XTB.PL PLN WHT 19%</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>11/01/2025 - 19/08/2025</t>
   </si>
 </sst>
 </file>
@@ -717,7 +750,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1065,9 +1098,6 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1089,9 +1119,6 @@
     <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1107,10 +1134,46 @@
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1127,52 +1190,40 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1899,14 +1950,14 @@
   </cols>
   <sheetData>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="141" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="142"/>
       <c r="H9" s="35" t="s">
         <v>1</v>
       </c>
@@ -1946,18 +1997,18 @@
       <c r="T9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U9" s="136"/>
-      <c r="V9" s="136"/>
-      <c r="W9" s="136"/>
-      <c r="X9" s="136"/>
+      <c r="U9" s="142"/>
+      <c r="V9" s="142"/>
+      <c r="W9" s="142"/>
+      <c r="X9" s="142"/>
     </row>
     <row r="10" spans="1:50" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="143" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="136"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
       <c r="F10" s="24" t="s">
         <v>1</v>
       </c>
@@ -2003,21 +2054,21 @@
       <c r="T10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="V10" s="136"/>
-      <c r="W10" s="136"/>
+      <c r="U10" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" s="142"/>
+      <c r="W10" s="142"/>
     </row>
     <row r="11" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="146" t="s">
+      <c r="B11" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="142"/>
+      <c r="E11" s="142"/>
+      <c r="F11" s="142"/>
+      <c r="G11" s="142"/>
       <c r="H11" s="24" t="s">
         <v>1</v>
       </c>
@@ -2057,11 +2108,11 @@
       <c r="T11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="V11" s="136"/>
-      <c r="W11" s="136"/>
+      <c r="U11" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" s="142"/>
+      <c r="W11" s="142"/>
     </row>
     <row r="12" spans="1:50" s="1" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A12" s="21"/>
@@ -2122,11 +2173,11 @@
       <c r="T12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U12" s="137" t="s">
+      <c r="U12" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="138"/>
-      <c r="W12" s="138"/>
+      <c r="V12" s="148"/>
+      <c r="W12" s="148"/>
       <c r="X12" s="21"/>
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
@@ -2211,11 +2262,11 @@
         <f>M13-L13</f>
         <v>135.65999999999997</v>
       </c>
-      <c r="U13" s="139" t="s">
-        <v>1</v>
-      </c>
-      <c r="V13" s="140"/>
-      <c r="W13" s="140"/>
+      <c r="U13" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="150"/>
+      <c r="W13" s="150"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
@@ -2299,11 +2350,11 @@
         <f t="shared" ref="T14:T16" si="2">M14-L14</f>
         <v>10</v>
       </c>
-      <c r="U14" s="141" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" s="142"/>
-      <c r="W14" s="142"/>
+      <c r="U14" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="152"/>
+      <c r="W14" s="152"/>
     </row>
     <row r="15" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
@@ -2361,11 +2412,11 @@
         <f t="shared" si="2"/>
         <v>-27.500000000000014</v>
       </c>
-      <c r="U15" s="139" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="140"/>
-      <c r="W15" s="140"/>
+      <c r="U15" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="150"/>
+      <c r="W15" s="150"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
@@ -2449,11 +2500,11 @@
         <f t="shared" si="2"/>
         <v>136.5</v>
       </c>
-      <c r="U16" s="141" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" s="142"/>
-      <c r="W16" s="142"/>
+      <c r="U16" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="152"/>
+      <c r="W16" s="152"/>
     </row>
     <row r="17" spans="2:23" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="32" t="s">
@@ -2514,26 +2565,26 @@
         <f>SUM(T13:T16)</f>
         <v>254.65999999999997</v>
       </c>
-      <c r="U17" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="V17" s="136"/>
-      <c r="W17" s="136"/>
+      <c r="U17" s="146" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="142"/>
+      <c r="W17" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="U9:X9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="U10:W10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2563,14 +2614,14 @@
   </cols>
   <sheetData>
     <row r="8" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
+      <c r="G8" s="142"/>
       <c r="H8" s="35" t="s">
         <v>1</v>
       </c>
@@ -2598,16 +2649,16 @@
       <c r="P8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="Q8" s="136"/>
-      <c r="R8" s="136"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="142"/>
     </row>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="147">
+      <c r="B9" s="153">
         <v>45713</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="147"/>
-      <c r="E9" s="147"/>
+      <c r="C9" s="153"/>
+      <c r="D9" s="153"/>
+      <c r="E9" s="153"/>
       <c r="F9" s="24" t="s">
         <v>1</v>
       </c>
@@ -3062,12 +3113,12 @@
   <sheetData>
     <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="143" t="s">
+      <c r="B9" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
       <c r="F9" s="35" t="s">
         <v>1</v>
       </c>
@@ -3089,17 +3140,17 @@
       <c r="L9" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="136"/>
-      <c r="N9" s="136"/>
+      <c r="M9" s="142"/>
+      <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:50" s="1" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
-      <c r="B10" s="148">
+      <c r="B10" s="154">
         <v>45713</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
       <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3221,10 +3272,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5EDB03-92D7-457B-986B-8E387DE2D6C9}">
-  <dimension ref="A19:AB55"/>
+  <dimension ref="A19:AB86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3240,27 +3291,27 @@
   </cols>
   <sheetData>
     <row r="19" spans="1:28" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="143" t="s">
+      <c r="B19" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="136"/>
-      <c r="D19" s="136"/>
-      <c r="E19" s="136"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="142"/>
       <c r="F19" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="136"/>
-      <c r="I19" s="136"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="142"/>
     </row>
     <row r="20" spans="1:28" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="144" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="136"/>
-      <c r="D20" s="136"/>
+      <c r="B20" s="143" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="142"/>
+      <c r="D20" s="142"/>
       <c r="E20" s="24" t="s">
         <v>1</v>
       </c>
@@ -3279,19 +3330,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H21" s="50" t="s">
         <v>1</v>
@@ -3493,7 +3544,7 @@
       <c r="G26" s="105">
         <v>1.01</v>
       </c>
-      <c r="H26" s="134" t="s">
+      <c r="H26" s="132" t="s">
         <v>1</v>
       </c>
       <c r="I26" s="89"/>
@@ -3537,7 +3588,7 @@
       <c r="G27" s="106">
         <v>-0.15</v>
       </c>
-      <c r="H27" s="134" t="s">
+      <c r="H27" s="132" t="s">
         <v>1</v>
       </c>
       <c r="I27" s="89"/>
@@ -3581,7 +3632,7 @@
       <c r="G28" s="105">
         <v>4.04</v>
       </c>
-      <c r="H28" s="134" t="s">
+      <c r="H28" s="132" t="s">
         <v>1</v>
       </c>
       <c r="I28" s="89"/>
@@ -3625,7 +3676,7 @@
       <c r="G29" s="106">
         <v>-0.61</v>
       </c>
-      <c r="H29" s="134" t="s">
+      <c r="H29" s="132" t="s">
         <v>1</v>
       </c>
       <c r="I29" s="89"/>
@@ -3661,7 +3712,7 @@
         <v>45669.453414351854</v>
       </c>
       <c r="E30" s="84" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="14">
@@ -3699,11 +3750,11 @@
       <c r="C31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="9">
-        <v>45709.465532407405</v>
+      <c r="D31" s="6">
+        <v>45669.453414351854</v>
       </c>
       <c r="E31" s="82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="17">
@@ -3745,7 +3796,7 @@
         <v>45668.639074074075</v>
       </c>
       <c r="E32" s="84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>27</v>
@@ -3839,7 +3890,7 @@
         <v>81</v>
       </c>
       <c r="G34" s="103">
-        <v>0.87</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="H34" s="50" t="s">
         <v>1</v>
@@ -3883,7 +3934,7 @@
         <v>81</v>
       </c>
       <c r="G35" s="104">
-        <v>-0.13</v>
+        <v>0.13</v>
       </c>
       <c r="H35" s="50" t="s">
         <v>1</v>
@@ -4097,7 +4148,7 @@
         <v>45701.158576388887</v>
       </c>
       <c r="E40" s="84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>27</v>
@@ -4141,7 +4192,7 @@
         <v>45705.054016203707</v>
       </c>
       <c r="E41" s="82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>40</v>
@@ -4185,7 +4236,7 @@
         <v>45683.412743055553</v>
       </c>
       <c r="E42" s="84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="18">
@@ -4227,7 +4278,7 @@
         <v>45678.173518518517</v>
       </c>
       <c r="E43" s="82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="17">
@@ -4269,7 +4320,7 @@
         <v>45704.304756944446</v>
       </c>
       <c r="E44" s="84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="14">
@@ -4311,7 +4362,7 @@
         <v>45679.018425925926</v>
       </c>
       <c r="E45" s="82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="46">
@@ -4386,22 +4437,22 @@
       <c r="AB46" s="21"/>
     </row>
     <row r="47" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="123">
+      <c r="B47" s="122">
         <v>315524141</v>
       </c>
-      <c r="C47" s="123" t="s">
+      <c r="C47" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="124">
+      <c r="D47" s="123">
         <v>45710.05940972222</v>
       </c>
-      <c r="E47" s="123" t="s">
+      <c r="E47" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="F47" s="125" t="s">
+      <c r="F47" s="124" t="s">
         <v>40</v>
       </c>
-      <c r="G47" s="126">
+      <c r="G47" s="125">
         <v>-255.6</v>
       </c>
       <c r="H47" s="50" t="s">
@@ -4460,7 +4511,7 @@
         <v>31</v>
       </c>
       <c r="D49" s="108">
-        <v>45443.500070046299</v>
+        <v>45808.500069444446</v>
       </c>
       <c r="E49" s="107" t="s">
         <v>86</v>
@@ -4469,7 +4520,7 @@
         <v>27</v>
       </c>
       <c r="G49" s="109">
-        <v>6.69</v>
+        <v>6.84</v>
       </c>
       <c r="H49" s="50"/>
     </row>
@@ -4482,16 +4533,16 @@
         <v>33</v>
       </c>
       <c r="D50" s="108">
-        <v>45443.500070046299</v>
-      </c>
-      <c r="E50" s="116" t="s">
+        <v>45808.500069444446</v>
+      </c>
+      <c r="E50" s="119" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="117" t="s">
         <v>27</v>
       </c>
       <c r="G50" s="118">
-        <v>-2.0099999999999998</v>
+        <v>-1.03</v>
       </c>
       <c r="H50" s="50"/>
       <c r="I50" s="21"/>
@@ -4516,23 +4567,23 @@
       <c r="AB50" s="21"/>
     </row>
     <row r="51" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="127">
+      <c r="B51" s="126">
         <v>89498937</v>
       </c>
-      <c r="C51" s="127" t="s">
+      <c r="C51" s="126" t="s">
         <v>31</v>
       </c>
       <c r="D51" s="108">
-        <v>45443.500070046299</v>
-      </c>
-      <c r="E51" s="127" t="s">
+        <v>45808.500069444446</v>
+      </c>
+      <c r="E51" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="F51" s="128" t="s">
+      <c r="F51" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="129">
-        <v>6.77</v>
+      <c r="G51" s="109">
+        <v>6.84</v>
       </c>
       <c r="H51" s="50"/>
     </row>
@@ -4545,16 +4596,16 @@
         <v>33</v>
       </c>
       <c r="D52" s="108">
-        <v>45443.500070046299</v>
+        <v>45808.500069444446</v>
       </c>
       <c r="E52" s="119" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F52" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="G52" s="121">
-        <v>-0.95</v>
+      <c r="G52" s="118">
+        <v>-1.03</v>
       </c>
       <c r="H52" s="50"/>
       <c r="I52" s="21"/>
@@ -4579,29 +4630,29 @@
       <c r="AB52" s="21"/>
     </row>
     <row r="53" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="130">
+      <c r="B53" s="128">
         <v>488088046</v>
       </c>
-      <c r="C53" s="127" t="s">
+      <c r="C53" s="126" t="s">
         <v>31</v>
       </c>
       <c r="D53" s="9">
         <v>45709.465532407405</v>
       </c>
-      <c r="E53" s="131" t="s">
+      <c r="E53" s="129" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="F53" s="132" t="s">
-        <v>90</v>
-      </c>
-      <c r="G53" s="133">
-        <v>3.91</v>
+      <c r="G53" s="131">
+        <v>4.2</v>
       </c>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="21"/>
-      <c r="B54" s="122">
+      <c r="B54" s="121">
         <v>138150122</v>
       </c>
       <c r="C54" s="119" t="s">
@@ -4611,13 +4662,13 @@
         <v>45709.465532407405</v>
       </c>
       <c r="E54" s="116" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" s="117" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G54" s="118">
-        <v>-0.14000000000000001</v>
+        <v>-1.26</v>
       </c>
       <c r="H54" s="50"/>
       <c r="I54" s="21"/>
@@ -4641,27 +4692,723 @@
       <c r="AA54" s="21"/>
       <c r="AB54" s="21"/>
     </row>
-    <row r="55" spans="1:28" s="21" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="32" t="s">
+    <row r="55" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="21"/>
+      <c r="B55" s="133">
+        <v>582941037</v>
+      </c>
+      <c r="C55" s="133" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="134">
+        <v>45895.670243055552</v>
+      </c>
+      <c r="E55" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="139" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" s="135">
+        <v>1.17</v>
+      </c>
+      <c r="H55" s="50"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21"/>
+      <c r="Q55" s="21"/>
+      <c r="R55" s="21"/>
+      <c r="S55" s="21"/>
+      <c r="T55" s="21"/>
+      <c r="U55" s="21"/>
+      <c r="V55" s="21"/>
+      <c r="W55" s="21"/>
+      <c r="X55" s="21"/>
+      <c r="Y55" s="21"/>
+      <c r="Z55" s="21"/>
+      <c r="AA55" s="21"/>
+      <c r="AB55" s="21"/>
+    </row>
+    <row r="56" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="21"/>
+      <c r="B56" s="136">
+        <v>104729583</v>
+      </c>
+      <c r="C56" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="137">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E56" s="136" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="G56" s="138">
+        <v>-0.32</v>
+      </c>
+      <c r="H56" s="50"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21"/>
+      <c r="R56" s="21"/>
+      <c r="S56" s="21"/>
+      <c r="T56" s="21"/>
+      <c r="U56" s="21"/>
+      <c r="V56" s="21"/>
+      <c r="W56" s="21"/>
+      <c r="X56" s="21"/>
+      <c r="Y56" s="21"/>
+      <c r="Z56" s="21"/>
+      <c r="AA56" s="21"/>
+      <c r="AB56" s="21"/>
+    </row>
+    <row r="57" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="21"/>
+      <c r="B57" s="133">
+        <v>672104958</v>
+      </c>
+      <c r="C57" s="133" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="134">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E57" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="139" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57" s="135">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H57" s="50"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
+      <c r="Q57" s="21"/>
+      <c r="R57" s="21"/>
+      <c r="S57" s="21"/>
+      <c r="T57" s="21"/>
+      <c r="U57" s="21"/>
+      <c r="V57" s="21"/>
+      <c r="W57" s="21"/>
+      <c r="X57" s="21"/>
+      <c r="Y57" s="21"/>
+      <c r="Z57" s="21"/>
+      <c r="AA57" s="21"/>
+      <c r="AB57" s="21"/>
+    </row>
+    <row r="58" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="21"/>
+      <c r="B58" s="136">
+        <v>394857126</v>
+      </c>
+      <c r="C58" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="137">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E58" s="136" t="s">
+        <v>106</v>
+      </c>
+      <c r="F58" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="G58" s="138">
+        <v>-0.16</v>
+      </c>
+      <c r="H58" s="50"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="21"/>
+      <c r="R58" s="21"/>
+      <c r="S58" s="21"/>
+      <c r="T58" s="21"/>
+      <c r="U58" s="21"/>
+      <c r="V58" s="21"/>
+      <c r="W58" s="21"/>
+      <c r="X58" s="21"/>
+      <c r="Y58" s="21"/>
+      <c r="Z58" s="21"/>
+      <c r="AA58" s="21"/>
+      <c r="AB58" s="21"/>
+    </row>
+    <row r="59" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="21"/>
+      <c r="B59" s="5">
+        <v>827364501</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="6">
+        <v>45806.4937884838</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G59" s="14">
+        <v>22.43</v>
+      </c>
+      <c r="H59" s="50"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21"/>
+      <c r="Q59" s="21"/>
+      <c r="R59" s="21"/>
+      <c r="S59" s="21"/>
+      <c r="T59" s="21"/>
+      <c r="U59" s="21"/>
+      <c r="V59" s="21"/>
+      <c r="W59" s="21"/>
+      <c r="X59" s="21"/>
+      <c r="Y59" s="21"/>
+      <c r="Z59" s="21"/>
+      <c r="AA59" s="21"/>
+      <c r="AB59" s="21"/>
+    </row>
+    <row r="60" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="21"/>
+      <c r="B60" s="8">
+        <v>210948573</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="9">
+        <v>45806.493810161999</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G60" s="46">
+        <v>28.03</v>
+      </c>
+      <c r="H60" s="50"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
+      <c r="Q60" s="21"/>
+      <c r="R60" s="21"/>
+      <c r="S60" s="21"/>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
+      <c r="V60" s="21"/>
+      <c r="W60" s="21"/>
+      <c r="X60" s="21"/>
+      <c r="Y60" s="21"/>
+      <c r="Z60" s="21"/>
+      <c r="AA60" s="21"/>
+      <c r="AB60" s="21"/>
+    </row>
+    <row r="61" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="21"/>
+      <c r="B61" s="5">
+        <v>746352910</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="6">
+        <v>45806.493816539398</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G61" s="14">
+        <v>44.85</v>
+      </c>
+      <c r="H61" s="50"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="21"/>
+      <c r="Q61" s="21"/>
+      <c r="R61" s="21"/>
+      <c r="S61" s="21"/>
+      <c r="T61" s="21"/>
+      <c r="U61" s="21"/>
+      <c r="V61" s="21"/>
+      <c r="W61" s="21"/>
+      <c r="X61" s="21"/>
+      <c r="Y61" s="21"/>
+      <c r="Z61" s="21"/>
+      <c r="AA61" s="21"/>
+      <c r="AB61" s="21"/>
+    </row>
+    <row r="62" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="21"/>
+      <c r="B62" s="5">
+        <v>501928374</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="6">
+        <v>45888.497956736101</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G62" s="14">
+        <v>4.22</v>
+      </c>
+      <c r="H62" s="50"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="21"/>
+      <c r="P62" s="21"/>
+      <c r="Q62" s="21"/>
+      <c r="R62" s="21"/>
+      <c r="S62" s="21"/>
+      <c r="T62" s="21"/>
+      <c r="U62" s="21"/>
+      <c r="V62" s="21"/>
+      <c r="W62" s="21"/>
+      <c r="X62" s="21"/>
+      <c r="Y62" s="21"/>
+      <c r="Z62" s="21"/>
+      <c r="AA62" s="21"/>
+      <c r="AB62" s="21"/>
+    </row>
+    <row r="63" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="21"/>
+      <c r="B63" s="8">
+        <v>883746521</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="9">
+        <v>45888.497956747698</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G63" s="17">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="H63" s="50"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="21"/>
+      <c r="O63" s="21"/>
+      <c r="P63" s="21"/>
+      <c r="Q63" s="21"/>
+      <c r="R63" s="21"/>
+      <c r="S63" s="21"/>
+      <c r="T63" s="21"/>
+      <c r="U63" s="21"/>
+      <c r="V63" s="21"/>
+      <c r="W63" s="21"/>
+      <c r="X63" s="21"/>
+      <c r="Y63" s="21"/>
+      <c r="Z63" s="21"/>
+      <c r="AA63" s="21"/>
+      <c r="AB63" s="21"/>
+    </row>
+    <row r="64" spans="1:28" s="21" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="5">
+        <v>192837465</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="6">
+        <v>45888.497970567099</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G64" s="14">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="8">
+        <v>657483920</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="9">
+        <v>45888.497970567099</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G65" s="17">
+        <v>-1.71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="5">
+        <v>435261709</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="6">
+        <v>45888.497985914299</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G66" s="14">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="8">
+        <v>901827364</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="9">
+        <v>45888.497986111113</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G67" s="17">
+        <v>-2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="5">
+        <v>273645109</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="6">
+        <v>45888.497991967597</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G68" s="14">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" s="8">
+        <v>510293847</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="9">
+        <v>45888.497991979202</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G69" s="17">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B70" s="5">
+        <v>647583920</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="6">
+        <v>45888.498006701397</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G70" s="14">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B71" s="8">
+        <v>384756291</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" s="9">
+        <v>45888.498006713002</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G71" s="17">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B72" s="8">
+        <v>726354810</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="9">
+        <v>45833.328140034697</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G72" s="46">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B73" s="5">
+        <v>819203746</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="6">
+        <v>45833.328140034697</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" s="18">
+        <v>-8.2799999999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B74" s="8">
+        <v>152637489</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="9">
+        <v>45833.3282088079</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G74" s="46">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B75" s="5">
+        <v>948576102</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D75" s="6">
+        <v>45833.3282088079</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G75" s="18">
+        <v>-4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B76" s="8">
+        <v>203948576</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D76" s="9">
+        <v>45833.328220092597</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G76" s="46">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B77" s="5">
+        <v>475869201</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D77" s="6">
+        <v>45833.328220092597</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G77" s="18">
+        <v>-5.18</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B78" s="8">
+        <v>364758291</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D78" s="9">
+        <v>45833.3284321065</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G78" s="46">
+        <v>38.15</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B79" s="8">
+        <v>657483926</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" s="6">
+        <v>45833.3284321065</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G79" s="18">
+        <v>-7.25</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B80" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F55" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="G55" s="33">
-        <f>SUM(G22:G54)</f>
-        <v>-74.279999999999973</v>
-      </c>
-      <c r="H55" s="51" t="s">
+      <c r="F80" s="51"/>
+      <c r="G80" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="H80" s="51" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="33"/>
+      <c r="H86" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4729,16 +5476,16 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:38" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="141" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
       <c r="J4" s="35" t="s">
         <v>1</v>
       </c>
@@ -4766,20 +5513,20 @@
       <c r="R4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="136"/>
-      <c r="T4" s="136"/>
-      <c r="U4" s="136"/>
-      <c r="V4" s="136"/>
+      <c r="S4" s="142"/>
+      <c r="T4" s="142"/>
+      <c r="U4" s="142"/>
+      <c r="V4" s="142"/>
     </row>
     <row r="5" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
       <c r="H5" s="24" t="s">
         <v>1</v>
       </c>
@@ -4813,23 +5560,23 @@
       <c r="R5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="T5" s="136"/>
-      <c r="U5" s="136"/>
+      <c r="S5" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="142"/>
+      <c r="U5" s="142"/>
     </row>
     <row r="6" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="146" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
-      <c r="I6" s="136"/>
+      <c r="B6" s="145" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
+      <c r="I6" s="142"/>
       <c r="J6" s="24" t="s">
         <v>1</v>
       </c>
@@ -4857,21 +5604,21 @@
       <c r="R6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" s="136"/>
-      <c r="U6" s="136"/>
+      <c r="S6" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="142"/>
+      <c r="U6" s="142"/>
     </row>
     <row r="7" spans="1:38" s="21" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="156" t="s">
+      <c r="B7" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="157" t="s">
+      <c r="C7" s="142"/>
+      <c r="D7" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="136"/>
+      <c r="E7" s="142"/>
       <c r="F7" s="25" t="s">
         <v>3</v>
       </c>
@@ -4911,22 +5658,22 @@
       <c r="R7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="157" t="s">
-        <v>1</v>
-      </c>
-      <c r="T7" s="136"/>
-      <c r="U7" s="136"/>
+      <c r="S7" s="164" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" s="142"/>
+      <c r="U7" s="142"/>
     </row>
     <row r="8" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
-      <c r="B8" s="139">
+      <c r="B8" s="149">
         <v>442606945</v>
       </c>
-      <c r="C8" s="140"/>
-      <c r="D8" s="158" t="s">
+      <c r="C8" s="150"/>
+      <c r="D8" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="140"/>
+      <c r="E8" s="150"/>
       <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
@@ -4967,11 +5714,11 @@
       <c r="R8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="155" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="152"/>
-      <c r="U8" s="152"/>
+      <c r="S8" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="157"/>
+      <c r="U8" s="157"/>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
@@ -4992,14 +5739,14 @@
     </row>
     <row r="9" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
-      <c r="B9" s="149">
+      <c r="B9" s="158">
         <v>654595998</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="150" t="s">
+      <c r="C9" s="150"/>
+      <c r="D9" s="159" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="150"/>
+      <c r="E9" s="159"/>
       <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
@@ -5040,11 +5787,11 @@
       <c r="R9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="151" t="s">
-        <v>1</v>
-      </c>
-      <c r="T9" s="152"/>
-      <c r="U9" s="152"/>
+      <c r="S9" s="160" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="157"/>
+      <c r="U9" s="157"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
@@ -5065,14 +5812,14 @@
     </row>
     <row r="10" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
-      <c r="B10" s="139">
+      <c r="B10" s="149">
         <v>620339720</v>
       </c>
-      <c r="C10" s="140"/>
-      <c r="D10" s="153" t="s">
+      <c r="C10" s="150"/>
+      <c r="D10" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="154"/>
+      <c r="E10" s="162"/>
       <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5113,11 +5860,11 @@
       <c r="R10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="155" t="s">
-        <v>1</v>
-      </c>
-      <c r="T10" s="152"/>
-      <c r="U10" s="152"/>
+      <c r="S10" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
@@ -5137,14 +5884,14 @@
       <c r="AL10" s="21"/>
     </row>
     <row r="11" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="136"/>
-      <c r="D11" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="136"/>
+      <c r="C11" s="142"/>
+      <c r="D11" s="146" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="142"/>
       <c r="F11" s="32" t="s">
         <v>1</v>
       </c>
@@ -5183,22 +5930,17 @@
       <c r="R11" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="T11" s="136"/>
-      <c r="U11" s="136"/>
+      <c r="S11" s="146" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="142"/>
+      <c r="U11" s="142"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="H12" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="S5:U5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="S11:U11"/>
@@ -5215,6 +5957,11 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5225,8 +5972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1BF635-54CB-4B79-8A30-07ED0777253E}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5268,27 +6015,27 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:29" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
       <c r="F4" s="35" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
     </row>
     <row r="5" spans="1:29" s="21" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
       <c r="E5" s="24" t="s">
         <v>1</v>
       </c>
@@ -5530,7 +6277,7 @@
     </row>
     <row r="12" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="39">
-        <v>1803</v>
+        <v>180342422</v>
       </c>
       <c r="C12" s="39" t="s">
         <v>9</v>
@@ -5962,7 +6709,7 @@
     <row r="25" spans="1:29" s="83" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="89"/>
       <c r="B25" s="97">
-        <v>2519363</v>
+        <v>251936333</v>
       </c>
       <c r="C25" s="97" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Enhance tax rate extraction from dividend comments
Updated DataFrameProcessor to extract tax rates from the 'Comment' field (e.g., 'WHT 27%') before falling back to default rates based on ticker.
</commit_message>
<xml_diff>
--- a/data/demo_XTB_broker_statement.xlsx
+++ b/data/demo_XTB_broker_statement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wojci\OneDrive\Dokumenty\GitHub\xtb-dividend-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FFD52B-876F-4ADA-B7EC-6368539DE120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE4043-09A4-4E86-A1AC-C540A40E3387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6735" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
+    <workbookView xWindow="57435" yWindow="6690" windowWidth="29130" windowHeight="15810" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
   </bookViews>
   <sheets>
     <sheet name="CLOSED POSITION HISTORY" sheetId="1" r:id="rId1"/>
@@ -1158,10 +1158,29 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1171,59 +1190,40 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1950,7 +1950,7 @@
   </cols>
   <sheetData>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="149" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="142"/>
@@ -2003,7 +2003,7 @@
       <c r="X9" s="142"/>
     </row>
     <row r="10" spans="1:50" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="143" t="s">
+      <c r="B10" s="150" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="142"/>
@@ -2054,14 +2054,14 @@
       <c r="T10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="144" t="s">
+      <c r="U10" s="151" t="s">
         <v>1</v>
       </c>
       <c r="V10" s="142"/>
       <c r="W10" s="142"/>
     </row>
     <row r="11" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="145" t="s">
+      <c r="B11" s="152" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="142"/>
@@ -2108,7 +2108,7 @@
       <c r="T11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="144" t="s">
+      <c r="U11" s="151" t="s">
         <v>1</v>
       </c>
       <c r="V11" s="142"/>
@@ -2173,11 +2173,11 @@
       <c r="T12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U12" s="147" t="s">
+      <c r="U12" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="148"/>
-      <c r="W12" s="148"/>
+      <c r="V12" s="144"/>
+      <c r="W12" s="144"/>
       <c r="X12" s="21"/>
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
@@ -2262,11 +2262,11 @@
         <f>M13-L13</f>
         <v>135.65999999999997</v>
       </c>
-      <c r="U13" s="149" t="s">
-        <v>1</v>
-      </c>
-      <c r="V13" s="150"/>
-      <c r="W13" s="150"/>
+      <c r="U13" s="145" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="146"/>
+      <c r="W13" s="146"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
@@ -2350,11 +2350,11 @@
         <f t="shared" ref="T14:T16" si="2">M14-L14</f>
         <v>10</v>
       </c>
-      <c r="U14" s="151" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" s="152"/>
-      <c r="W14" s="152"/>
+      <c r="U14" s="147" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="148"/>
+      <c r="W14" s="148"/>
     </row>
     <row r="15" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
@@ -2412,11 +2412,11 @@
         <f t="shared" si="2"/>
         <v>-27.500000000000014</v>
       </c>
-      <c r="U15" s="149" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="150"/>
-      <c r="W15" s="150"/>
+      <c r="U15" s="145" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="146"/>
+      <c r="W15" s="146"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
@@ -2500,11 +2500,11 @@
         <f t="shared" si="2"/>
         <v>136.5</v>
       </c>
-      <c r="U16" s="151" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" s="152"/>
-      <c r="W16" s="152"/>
+      <c r="U16" s="147" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="148"/>
+      <c r="W16" s="148"/>
     </row>
     <row r="17" spans="2:23" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="32" t="s">
@@ -2565,7 +2565,7 @@
         <f>SUM(T13:T16)</f>
         <v>254.65999999999997</v>
       </c>
-      <c r="U17" s="146" t="s">
+      <c r="U17" s="141" t="s">
         <v>1</v>
       </c>
       <c r="V17" s="142"/>
@@ -2573,18 +2573,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="U11:W11"/>
     <mergeCell ref="U17:W17"/>
     <mergeCell ref="U12:W12"/>
     <mergeCell ref="U13:W13"/>
     <mergeCell ref="U14:W14"/>
     <mergeCell ref="U15:W15"/>
     <mergeCell ref="U16:W16"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="U9:X9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="U11:W11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2614,7 +2614,7 @@
   </cols>
   <sheetData>
     <row r="8" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="149" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="142"/>
@@ -3113,7 +3113,7 @@
   <sheetData>
     <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="149" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="142"/>
@@ -3275,7 +3275,7 @@
   <dimension ref="A19:AB86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3291,7 +3291,7 @@
   </cols>
   <sheetData>
     <row r="19" spans="1:28" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="141" t="s">
+      <c r="B19" s="149" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="142"/>
@@ -3307,7 +3307,7 @@
       <c r="I19" s="142"/>
     </row>
     <row r="20" spans="1:28" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="150" t="s">
         <v>115</v>
       </c>
       <c r="C20" s="142"/>
@@ -4511,7 +4511,7 @@
         <v>31</v>
       </c>
       <c r="D49" s="108">
-        <v>45808.500069444446</v>
+        <v>45663.500069444446</v>
       </c>
       <c r="E49" s="107" t="s">
         <v>86</v>
@@ -4533,7 +4533,7 @@
         <v>33</v>
       </c>
       <c r="D50" s="108">
-        <v>45808.500069444446</v>
+        <v>45663.500069444446</v>
       </c>
       <c r="E50" s="119" t="s">
         <v>87</v>
@@ -5358,7 +5358,7 @@
         <v>80</v>
       </c>
       <c r="D78" s="9">
-        <v>45833.3284321065</v>
+        <v>45944.3284375</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>112</v>
@@ -5377,8 +5377,8 @@
       <c r="C79" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="6">
-        <v>45833.3284321065</v>
+      <c r="D79" s="9">
+        <v>45944.3284375</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>113</v>
@@ -5476,7 +5476,7 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:38" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="149" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="142"/>
@@ -5519,7 +5519,7 @@
       <c r="V4" s="142"/>
     </row>
     <row r="5" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="150" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="142"/>
@@ -5560,14 +5560,14 @@
       <c r="R5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="144" t="s">
+      <c r="S5" s="151" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="142"/>
       <c r="U5" s="142"/>
     </row>
     <row r="6" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="152" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="142"/>
@@ -5604,18 +5604,18 @@
       <c r="R6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="144" t="s">
+      <c r="S6" s="151" t="s">
         <v>1</v>
       </c>
       <c r="T6" s="142"/>
       <c r="U6" s="142"/>
     </row>
     <row r="7" spans="1:38" s="21" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="163" t="s">
+      <c r="B7" s="162" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="142"/>
-      <c r="D7" s="164" t="s">
+      <c r="D7" s="163" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="142"/>
@@ -5658,7 +5658,7 @@
       <c r="R7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="164" t="s">
+      <c r="S7" s="163" t="s">
         <v>1</v>
       </c>
       <c r="T7" s="142"/>
@@ -5666,14 +5666,14 @@
     </row>
     <row r="8" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
-      <c r="B8" s="149">
+      <c r="B8" s="145">
         <v>442606945</v>
       </c>
-      <c r="C8" s="150"/>
-      <c r="D8" s="155" t="s">
+      <c r="C8" s="146"/>
+      <c r="D8" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="150"/>
+      <c r="E8" s="146"/>
       <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
@@ -5714,11 +5714,11 @@
       <c r="R8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="156" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="157"/>
-      <c r="U8" s="157"/>
+      <c r="S8" s="161" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="158"/>
+      <c r="U8" s="158"/>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
@@ -5739,14 +5739,14 @@
     </row>
     <row r="9" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
-      <c r="B9" s="158">
+      <c r="B9" s="155">
         <v>654595998</v>
       </c>
-      <c r="C9" s="150"/>
-      <c r="D9" s="159" t="s">
+      <c r="C9" s="146"/>
+      <c r="D9" s="156" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="159"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
@@ -5787,11 +5787,11 @@
       <c r="R9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="160" t="s">
-        <v>1</v>
-      </c>
-      <c r="T9" s="157"/>
-      <c r="U9" s="157"/>
+      <c r="S9" s="157" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="158"/>
+      <c r="U9" s="158"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
@@ -5812,14 +5812,14 @@
     </row>
     <row r="10" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
-      <c r="B10" s="149">
+      <c r="B10" s="145">
         <v>620339720</v>
       </c>
-      <c r="C10" s="150"/>
-      <c r="D10" s="161" t="s">
+      <c r="C10" s="146"/>
+      <c r="D10" s="159" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="162"/>
+      <c r="E10" s="160"/>
       <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5860,11 +5860,11 @@
       <c r="R10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="156" t="s">
-        <v>1</v>
-      </c>
-      <c r="T10" s="157"/>
-      <c r="U10" s="157"/>
+      <c r="S10" s="161" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="158"/>
+      <c r="U10" s="158"/>
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
@@ -5884,11 +5884,11 @@
       <c r="AL10" s="21"/>
     </row>
     <row r="11" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="146" t="s">
+      <c r="B11" s="141" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="142"/>
-      <c r="D11" s="146" t="s">
+      <c r="D11" s="141" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="142"/>
@@ -5930,7 +5930,7 @@
       <c r="R11" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="146" t="s">
+      <c r="S11" s="141" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="142"/>
@@ -5941,6 +5941,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="S11:U11"/>
@@ -5957,11 +5962,6 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6015,7 +6015,7 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:29" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="149" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="142"/>
@@ -6031,7 +6031,7 @@
       <c r="I4" s="142"/>
     </row>
     <row r="5" spans="1:29" s="21" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="150" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="142"/>

</xml_diff>

<commit_message>
Add Date D-1 and Exchange Rate D-1 columns
- Add 'Date D-1' column showing previous business day from dividend date
  - Automatically skips weekends (Saturday/Sunday) to find last weekday
  - Handles pandas Timestamp and datetime objects

- Add 'Exchange Rate D-1' column with exchange rates for D-1 dates
  - Extracts currency from Net Dividend column (USD, PLN, EUR, DKK, GBP)
  - Fetches exchange rate from archiwum_tab_a_*.csv for D-1 date
  - Shows "-" for PLN (base currency)
  - Formats rates with 4 decimal places

- Update column ordering to include new columns after Tax Collected %
- Import timedelta for date calculations
- Update exchange rate data (archiwum_tab_a_2025.csv)

Example: Dividend on 2025-01-06 (Monday) → D-1 = 2025-01-03 (Friday)
because Jan 4-5 was weekend
</commit_message>
<xml_diff>
--- a/data/demo_XTB_broker_statement.xlsx
+++ b/data/demo_XTB_broker_statement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wojci\OneDrive\Dokumenty\GitHub\xtb-dividend-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE4043-09A4-4E86-A1AC-C540A40E3387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213D6FE-C55E-4CBB-A9D0-3C3333CE9B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57435" yWindow="6690" windowWidth="29130" windowHeight="15810" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
+    <workbookView xWindow="57480" yWindow="6735" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{161875ED-7931-4FB8-A1C3-8F22BD6926D1}"/>
   </bookViews>
   <sheets>
     <sheet name="CLOSED POSITION HISTORY" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="124">
   <si>
     <r>
       <rPr>
@@ -485,6 +485,30 @@
   </si>
   <si>
     <t>11/01/2025 - 19/08/2025</t>
+  </si>
+  <si>
+    <t>Name and surname</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Free margin</t>
+  </si>
+  <si>
+    <t>Margin level</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -750,7 +774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1158,10 +1182,22 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1178,53 +1214,60 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1391,13 +1434,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1473200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>515761</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1950,7 +1993,7 @@
   </cols>
   <sheetData>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="141" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="142"/>
@@ -2003,7 +2046,7 @@
       <c r="X9" s="142"/>
     </row>
     <row r="10" spans="1:50" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="143" t="s">
         <v>66</v>
       </c>
       <c r="C10" s="142"/>
@@ -2054,14 +2097,14 @@
       <c r="T10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U10" s="151" t="s">
+      <c r="U10" s="144" t="s">
         <v>1</v>
       </c>
       <c r="V10" s="142"/>
       <c r="W10" s="142"/>
     </row>
     <row r="11" spans="1:50" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="145" t="s">
         <v>68</v>
       </c>
       <c r="C11" s="142"/>
@@ -2108,7 +2151,7 @@
       <c r="T11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="151" t="s">
+      <c r="U11" s="144" t="s">
         <v>1</v>
       </c>
       <c r="V11" s="142"/>
@@ -2173,11 +2216,11 @@
       <c r="T12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="U12" s="143" t="s">
+      <c r="U12" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="144"/>
-      <c r="W12" s="144"/>
+      <c r="V12" s="148"/>
+      <c r="W12" s="148"/>
       <c r="X12" s="21"/>
       <c r="Y12" s="21"/>
       <c r="Z12" s="21"/>
@@ -2262,11 +2305,11 @@
         <f>M13-L13</f>
         <v>135.65999999999997</v>
       </c>
-      <c r="U13" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="V13" s="146"/>
-      <c r="W13" s="146"/>
+      <c r="U13" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" s="150"/>
+      <c r="W13" s="150"/>
       <c r="X13" s="21"/>
       <c r="Y13" s="21"/>
       <c r="Z13" s="21"/>
@@ -2350,11 +2393,11 @@
         <f t="shared" ref="T14:T16" si="2">M14-L14</f>
         <v>10</v>
       </c>
-      <c r="U14" s="147" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" s="148"/>
-      <c r="W14" s="148"/>
+      <c r="U14" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="152"/>
+      <c r="W14" s="152"/>
     </row>
     <row r="15" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
@@ -2412,11 +2455,11 @@
         <f t="shared" si="2"/>
         <v>-27.500000000000014</v>
       </c>
-      <c r="U15" s="145" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="146"/>
-      <c r="W15" s="146"/>
+      <c r="U15" s="149" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="150"/>
+      <c r="W15" s="150"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
       <c r="Z15" s="21"/>
@@ -2500,11 +2543,11 @@
         <f t="shared" si="2"/>
         <v>136.5</v>
       </c>
-      <c r="U16" s="147" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" s="148"/>
-      <c r="W16" s="148"/>
+      <c r="U16" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="152"/>
+      <c r="W16" s="152"/>
     </row>
     <row r="17" spans="2:23" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="32" t="s">
@@ -2565,7 +2608,7 @@
         <f>SUM(T13:T16)</f>
         <v>254.65999999999997</v>
       </c>
-      <c r="U17" s="141" t="s">
+      <c r="U17" s="146" t="s">
         <v>1</v>
       </c>
       <c r="V17" s="142"/>
@@ -2573,18 +2616,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="U9:X9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="U10:W10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2614,7 +2657,7 @@
   </cols>
   <sheetData>
     <row r="8" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="149" t="s">
+      <c r="B8" s="141" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="142"/>
@@ -3113,7 +3156,7 @@
   <sheetData>
     <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:50" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="141" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="142"/>
@@ -3272,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5EDB03-92D7-457B-986B-8E387DE2D6C9}">
-  <dimension ref="A19:AB86"/>
+  <dimension ref="A5:AB76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3290,83 +3333,561 @@
     <col min="8" max="16384" width="8.7265625" style="34"/>
   </cols>
   <sheetData>
-    <row r="19" spans="1:28" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="149" t="s">
+    <row r="5" spans="1:28" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="165" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="166" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="166" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="166" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="171" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="167" customFormat="1" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="168" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="169" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="170" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="170" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="170" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="170" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="142"/>
-      <c r="I19" s="142"/>
-    </row>
-    <row r="20" spans="1:28" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="150" t="s">
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="142"/>
+      <c r="I9" s="142"/>
+    </row>
+    <row r="10" spans="1:28" s="21" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="3" t="s">
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="H11" s="50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="5">
+        <v>294997602</v>
+      </c>
+      <c r="C12" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45709.007928240739</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="14">
+        <v>11.62</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+    </row>
+    <row r="13" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="8">
+        <v>508873093</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6">
+        <v>45709.007928240739</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="17">
+        <v>-2.21</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
+    </row>
+    <row r="14" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="5">
+        <v>937654529</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6">
+        <v>45709.007928240739</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="14">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="21"/>
+      <c r="AA14" s="21"/>
+      <c r="AB14" s="21"/>
+    </row>
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="8">
+        <v>544055056</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="6">
+        <v>45709.007928240739</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="17">
+        <v>-3.15</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="21"/>
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+    </row>
+    <row r="16" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="89"/>
+      <c r="B16" s="82">
+        <v>762058528</v>
+      </c>
+      <c r="C16" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="87">
+        <v>45747.453486620398</v>
+      </c>
+      <c r="E16" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="105">
+        <v>1.01</v>
+      </c>
+      <c r="H16" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="89"/>
+      <c r="Q16" s="89"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="89"/>
+      <c r="T16" s="89"/>
+      <c r="U16" s="89"/>
+      <c r="V16" s="89"/>
+      <c r="W16" s="89"/>
+      <c r="X16" s="89"/>
+      <c r="Y16" s="89"/>
+      <c r="Z16" s="89"/>
+      <c r="AA16" s="89"/>
+      <c r="AB16" s="89"/>
+    </row>
+    <row r="17" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="89"/>
+      <c r="B17" s="84">
+        <v>762058529</v>
+      </c>
+      <c r="C17" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="85">
+        <v>45747.453486620398</v>
+      </c>
+      <c r="E17" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="106">
+        <v>-0.15</v>
+      </c>
+      <c r="H17" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="89"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="89"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="89"/>
+      <c r="AB17" s="89"/>
+    </row>
+    <row r="18" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="89"/>
+      <c r="B18" s="82">
+        <v>762065078</v>
+      </c>
+      <c r="C18" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="87">
+        <v>45747.453494745401</v>
+      </c>
+      <c r="E18" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="105">
+        <v>4.04</v>
+      </c>
+      <c r="H18" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
+      <c r="Q18" s="89"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="89"/>
+      <c r="T18" s="89"/>
+      <c r="U18" s="89"/>
+      <c r="V18" s="89"/>
+      <c r="W18" s="89"/>
+      <c r="X18" s="89"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="89"/>
+      <c r="AB18" s="89"/>
+    </row>
+    <row r="19" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="89"/>
+      <c r="B19" s="84">
+        <v>762065079</v>
+      </c>
+      <c r="C19" s="84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="85">
+        <v>45747.453494745401</v>
+      </c>
+      <c r="E19" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="106">
+        <v>-0.61</v>
+      </c>
+      <c r="H19" s="132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="89"/>
+      <c r="J19" s="89"/>
+      <c r="K19" s="89"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="89"/>
+      <c r="O19" s="89"/>
+      <c r="P19" s="89"/>
+      <c r="Q19" s="89"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="89"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="89"/>
+      <c r="V19" s="89"/>
+      <c r="W19" s="89"/>
+      <c r="X19" s="89"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="89"/>
+      <c r="AB19" s="89"/>
+    </row>
+    <row r="20" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="21"/>
+      <c r="B20" s="5">
+        <v>408822412</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="6">
+        <v>45669.453414351854</v>
+      </c>
+      <c r="E20" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="21"/>
+    </row>
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="21"/>
+      <c r="B21" s="8">
+        <v>347421144</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="6">
+        <v>45669.453414351854</v>
+      </c>
+      <c r="E21" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="17">
+        <v>-0.03</v>
+      </c>
       <c r="H21" s="50" t="s">
         <v>1</v>
       </c>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="21"/>
+      <c r="AB21" s="21"/>
     </row>
     <row r="22" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
       <c r="B22" s="5">
-        <v>294997602</v>
-      </c>
-      <c r="C22" s="84" t="s">
-        <v>31</v>
+        <v>241196438</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="6">
-        <v>45709.007928240739</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>8</v>
+        <v>45668.639074074075</v>
+      </c>
+      <c r="E22" s="84" t="s">
+        <v>93</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G22" s="14">
-        <v>11.62</v>
+        <v>361.52</v>
       </c>
       <c r="H22" s="50" t="s">
         <v>1</v>
@@ -3395,22 +3916,22 @@
     <row r="23" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21"/>
       <c r="B23" s="8">
-        <v>508873093</v>
-      </c>
-      <c r="C23" s="82" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="6">
-        <v>45709.007928240739</v>
+        <v>198251944</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="9">
+        <v>45678.044259259259</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="17">
-        <v>-2.21</v>
+        <v>27</v>
+      </c>
+      <c r="G23" s="46">
+        <v>880.62</v>
       </c>
       <c r="H23" s="50" t="s">
         <v>1</v>
@@ -3439,22 +3960,22 @@
     <row r="24" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="5">
-        <v>937654529</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="6">
-        <v>45709.007928240739</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="14">
-        <v>16.600000000000001</v>
+        <v>251936304</v>
+      </c>
+      <c r="C24" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="85">
+        <v>45750.490316469899</v>
+      </c>
+      <c r="E24" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="103">
+        <v>0.86499999999999999</v>
       </c>
       <c r="H24" s="50" t="s">
         <v>1</v>
@@ -3483,22 +4004,22 @@
     <row r="25" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
       <c r="B25" s="8">
-        <v>544055056</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="6">
-        <v>45709.007928240739</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="17">
-        <v>-3.15</v>
+        <v>263346911</v>
+      </c>
+      <c r="C25" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="87">
+        <v>45750.490316481497</v>
+      </c>
+      <c r="E25" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="104">
+        <v>0.13</v>
       </c>
       <c r="H25" s="50" t="s">
         <v>1</v>
@@ -3524,199 +4045,201 @@
       <c r="AA25" s="21"/>
       <c r="AB25" s="21"/>
     </row>
-    <row r="26" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="89"/>
-      <c r="B26" s="82">
-        <v>762058528</v>
-      </c>
-      <c r="C26" s="82" t="s">
+    <row r="26" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+      <c r="B26" s="5">
+        <v>131822864</v>
+      </c>
+      <c r="C26" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="87">
-        <v>45747.453486620398</v>
-      </c>
-      <c r="E26" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="105">
-        <v>1.01</v>
-      </c>
-      <c r="H26" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" s="89"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="89"/>
-      <c r="L26" s="89"/>
-      <c r="M26" s="89"/>
-      <c r="N26" s="89"/>
-      <c r="O26" s="89"/>
-      <c r="P26" s="89"/>
-      <c r="Q26" s="89"/>
-      <c r="R26" s="89"/>
-      <c r="S26" s="89"/>
-      <c r="T26" s="89"/>
-      <c r="U26" s="89"/>
-      <c r="V26" s="89"/>
-      <c r="W26" s="89"/>
-      <c r="X26" s="89"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="89"/>
-      <c r="AB26" s="89"/>
-    </row>
-    <row r="27" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="89"/>
-      <c r="B27" s="84">
-        <v>762058529</v>
-      </c>
-      <c r="C27" s="84" t="s">
+      <c r="D26" s="85">
+        <v>45750.490374050903</v>
+      </c>
+      <c r="E26" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="103">
+        <v>3.89</v>
+      </c>
+      <c r="H26" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="21"/>
+      <c r="AA26" s="21"/>
+      <c r="AB26" s="21"/>
+    </row>
+    <row r="27" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="8">
+        <v>188503932</v>
+      </c>
+      <c r="C27" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="85">
-        <v>45747.453486620398</v>
-      </c>
-      <c r="E27" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="106">
-        <v>-0.15</v>
-      </c>
-      <c r="H27" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="89"/>
-      <c r="R27" s="89"/>
-      <c r="S27" s="89"/>
-      <c r="T27" s="89"/>
-      <c r="U27" s="89"/>
-      <c r="V27" s="89"/>
-      <c r="W27" s="89"/>
-      <c r="X27" s="89"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="89"/>
-      <c r="AB27" s="89"/>
-    </row>
-    <row r="28" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="89"/>
-      <c r="B28" s="82">
-        <v>762065078</v>
-      </c>
-      <c r="C28" s="82" t="s">
+      <c r="D27" s="87">
+        <v>45750.490374050903</v>
+      </c>
+      <c r="E27" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="104">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="H27" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="21"/>
+    </row>
+    <row r="28" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="B28" s="5">
+        <v>881888549</v>
+      </c>
+      <c r="C28" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="87">
-        <v>45747.453494745401</v>
-      </c>
-      <c r="E28" s="82" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="88" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="105">
-        <v>4.04</v>
-      </c>
-      <c r="H28" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="89"/>
-      <c r="O28" s="89"/>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="89"/>
-      <c r="R28" s="89"/>
-      <c r="S28" s="89"/>
-      <c r="T28" s="89"/>
-      <c r="U28" s="89"/>
-      <c r="V28" s="89"/>
-      <c r="W28" s="89"/>
-      <c r="X28" s="89"/>
-      <c r="Y28" s="89"/>
-      <c r="Z28" s="89"/>
-      <c r="AA28" s="89"/>
-      <c r="AB28" s="89"/>
-    </row>
-    <row r="29" spans="1:28" s="83" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="89"/>
-      <c r="B29" s="84">
-        <v>762065079</v>
-      </c>
-      <c r="C29" s="84" t="s">
+      <c r="D28" s="85">
+        <v>45750.490385069403</v>
+      </c>
+      <c r="E28" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="103">
+        <v>4.76</v>
+      </c>
+      <c r="H28" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="21"/>
+      <c r="AA28" s="21"/>
+      <c r="AB28" s="21"/>
+    </row>
+    <row r="29" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="8">
+        <v>702542628</v>
+      </c>
+      <c r="C29" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="85">
-        <v>45747.453494745401</v>
-      </c>
-      <c r="E29" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="106">
-        <v>-0.61</v>
-      </c>
-      <c r="H29" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="89"/>
-      <c r="N29" s="89"/>
-      <c r="O29" s="89"/>
-      <c r="P29" s="89"/>
-      <c r="Q29" s="89"/>
-      <c r="R29" s="89"/>
-      <c r="S29" s="89"/>
-      <c r="T29" s="89"/>
-      <c r="U29" s="89"/>
-      <c r="V29" s="89"/>
-      <c r="W29" s="89"/>
-      <c r="X29" s="89"/>
-      <c r="Y29" s="89"/>
-      <c r="Z29" s="89"/>
-      <c r="AA29" s="89"/>
-      <c r="AB29" s="89"/>
+      <c r="D29" s="87">
+        <v>45750.490385069403</v>
+      </c>
+      <c r="E29" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="104">
+        <v>-0.71</v>
+      </c>
+      <c r="H29" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="21"/>
+      <c r="Z29" s="21"/>
+      <c r="AA29" s="21"/>
+      <c r="AB29" s="21"/>
     </row>
     <row r="30" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21"/>
       <c r="B30" s="5">
-        <v>408822412</v>
+        <v>646118208</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D30" s="6">
-        <v>45669.453414351854</v>
+        <v>45701.158576388887</v>
       </c>
       <c r="E30" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="14">
-        <v>0.14000000000000001</v>
+        <v>94</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="18">
+        <v>-0.05</v>
       </c>
       <c r="H30" s="50" t="s">
         <v>1</v>
@@ -3745,20 +4268,22 @@
     <row r="31" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21"/>
       <c r="B31" s="8">
-        <v>347421144</v>
+        <v>917985910</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="6">
-        <v>45669.453414351854</v>
+        <v>39</v>
+      </c>
+      <c r="D31" s="9">
+        <v>45705.054016203707</v>
       </c>
       <c r="E31" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="10"/>
+        <v>97</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="G31" s="17">
-        <v>-0.03</v>
+        <v>-344.4</v>
       </c>
       <c r="H31" s="50" t="s">
         <v>1</v>
@@ -3787,22 +4312,20 @@
     <row r="32" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="21"/>
       <c r="B32" s="5">
-        <v>241196438</v>
+        <v>942293239</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="6">
-        <v>45668.639074074075</v>
+        <v>45683.412743055553</v>
       </c>
       <c r="E32" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="14">
-        <v>361.52</v>
+        <v>98</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="18">
+        <v>-0.87</v>
       </c>
       <c r="H32" s="50" t="s">
         <v>1</v>
@@ -3831,22 +4354,20 @@
     <row r="33" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="21"/>
       <c r="B33" s="8">
-        <v>198251944</v>
+        <v>669676129</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" s="9">
-        <v>45678.044259259259</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="46">
-        <v>880.62</v>
+        <v>45678.173518518517</v>
+      </c>
+      <c r="E33" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="17">
+        <v>-0.03</v>
       </c>
       <c r="H33" s="50" t="s">
         <v>1</v>
@@ -3875,22 +4396,20 @@
     <row r="34" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21"/>
       <c r="B34" s="5">
-        <v>251936304</v>
-      </c>
-      <c r="C34" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="85">
-        <v>45750.490316469899</v>
+        <v>986691851</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="6">
+        <v>45704.304756944446</v>
       </c>
       <c r="E34" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="103">
-        <v>0.86499999999999999</v>
+        <v>95</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="14">
+        <v>0.12</v>
       </c>
       <c r="H34" s="50" t="s">
         <v>1</v>
@@ -3919,22 +4438,20 @@
     <row r="35" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21"/>
       <c r="B35" s="8">
-        <v>263346911</v>
-      </c>
-      <c r="C35" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="87">
-        <v>45750.490316481497</v>
+        <v>738944960</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="9">
+        <v>45679.018425925926</v>
       </c>
       <c r="E35" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="104">
-        <v>0.13</v>
+        <v>99</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="46">
+        <v>4.54</v>
       </c>
       <c r="H35" s="50" t="s">
         <v>1</v>
@@ -3963,22 +4480,22 @@
     <row r="36" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="21"/>
       <c r="B36" s="5">
-        <v>131822864</v>
-      </c>
-      <c r="C36" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="85">
-        <v>45750.490374050903</v>
-      </c>
-      <c r="E36" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="103">
-        <v>3.89</v>
+        <v>355368767</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45682.153043981481</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="18">
+        <v>-258.39999999999998</v>
       </c>
       <c r="H36" s="50" t="s">
         <v>1</v>
@@ -4004,69 +4521,48 @@
       <c r="AA36" s="21"/>
       <c r="AB36" s="21"/>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
-      <c r="B37" s="8">
-        <v>188503932</v>
-      </c>
-      <c r="C37" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="87">
-        <v>45750.490374050903</v>
-      </c>
-      <c r="E37" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="104">
-        <v>-0.57999999999999996</v>
+    <row r="37" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="122">
+        <v>315524141</v>
+      </c>
+      <c r="C37" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="123">
+        <v>45710.05940972222</v>
+      </c>
+      <c r="E37" s="122" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="124" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="125">
+        <v>-255.6</v>
       </c>
       <c r="H37" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="21"/>
-      <c r="X37" s="21"/>
-      <c r="Y37" s="21"/>
-      <c r="Z37" s="21"/>
-      <c r="AA37" s="21"/>
-      <c r="AB37" s="21"/>
-    </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="21"/>
-      <c r="B38" s="5">
-        <v>881888549</v>
-      </c>
-      <c r="C38" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="85">
-        <v>45750.490385069403</v>
-      </c>
-      <c r="E38" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="G38" s="103">
-        <v>4.76</v>
+      <c r="B38" s="112">
+        <v>141056374</v>
+      </c>
+      <c r="C38" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="113">
+        <v>45687.295057870368</v>
+      </c>
+      <c r="E38" s="112" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="115">
+        <v>-511.36</v>
       </c>
       <c r="H38" s="50" t="s">
         <v>1</v>
@@ -4092,73 +4588,48 @@
       <c r="AA38" s="21"/>
       <c r="AB38" s="21"/>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="8">
-        <v>702542628</v>
-      </c>
-      <c r="C39" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="87">
-        <v>45750.490385069403</v>
-      </c>
-      <c r="E39" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="G39" s="104">
-        <v>-0.71</v>
-      </c>
-      <c r="H39" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="21"/>
-    </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="107">
+        <v>863763119</v>
+      </c>
+      <c r="C39" s="107" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="108">
+        <v>45663.500069444446</v>
+      </c>
+      <c r="E39" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="109">
+        <v>6.84</v>
+      </c>
+      <c r="H39" s="50"/>
+    </row>
+    <row r="40" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="21"/>
-      <c r="B40" s="5">
-        <v>646118208</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="6">
-        <v>45701.158576388887</v>
-      </c>
-      <c r="E40" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="7" t="s">
+      <c r="B40" s="116">
+        <v>264122037</v>
+      </c>
+      <c r="C40" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="108">
+        <v>45663.500069444446</v>
+      </c>
+      <c r="E40" s="119" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="G40" s="18">
-        <v>-0.05</v>
-      </c>
-      <c r="H40" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="G40" s="118">
+        <v>-1.03</v>
+      </c>
+      <c r="H40" s="50"/>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
@@ -4180,71 +4651,48 @@
       <c r="AA40" s="21"/>
       <c r="AB40" s="21"/>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="21"/>
-      <c r="B41" s="8">
-        <v>917985910</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="9">
-        <v>45705.054016203707</v>
-      </c>
-      <c r="E41" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G41" s="17">
-        <v>-344.4</v>
-      </c>
-      <c r="H41" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="21"/>
-      <c r="AA41" s="21"/>
-      <c r="AB41" s="21"/>
-    </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="126">
+        <v>89498937</v>
+      </c>
+      <c r="C41" s="126" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="108">
+        <v>45808.500069444446</v>
+      </c>
+      <c r="E41" s="126" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="109">
+        <v>6.84</v>
+      </c>
+      <c r="H41" s="50"/>
+    </row>
+    <row r="42" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="21"/>
-      <c r="B42" s="5">
-        <v>942293239</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="6">
-        <v>45683.412743055553</v>
-      </c>
-      <c r="E42" s="84" t="s">
-        <v>98</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="18">
-        <v>-0.87</v>
-      </c>
-      <c r="H42" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B42" s="119">
+        <v>765529925</v>
+      </c>
+      <c r="C42" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="108">
+        <v>45808.500069444446</v>
+      </c>
+      <c r="E42" s="119" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="118">
+        <v>-1.03</v>
+      </c>
+      <c r="H42" s="50"/>
       <c r="I42" s="21"/>
       <c r="J42" s="21"/>
       <c r="K42" s="21"/>
@@ -4266,69 +4714,48 @@
       <c r="AA42" s="21"/>
       <c r="AB42" s="21"/>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="21"/>
-      <c r="B43" s="8">
-        <v>669676129</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>35</v>
+    <row r="43" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="128">
+        <v>488088046</v>
+      </c>
+      <c r="C43" s="126" t="s">
+        <v>31</v>
       </c>
       <c r="D43" s="9">
-        <v>45678.173518518517</v>
-      </c>
-      <c r="E43" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="17">
-        <v>-0.03</v>
-      </c>
-      <c r="H43" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="21"/>
-      <c r="R43" s="21"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
-      <c r="V43" s="21"/>
-      <c r="W43" s="21"/>
-      <c r="X43" s="21"/>
-      <c r="Y43" s="21"/>
-      <c r="Z43" s="21"/>
-      <c r="AA43" s="21"/>
-      <c r="AB43" s="21"/>
-    </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>45709.465532407405</v>
+      </c>
+      <c r="E43" s="129" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="130" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="131">
+        <v>4.2</v>
+      </c>
+      <c r="H43" s="50"/>
+    </row>
+    <row r="44" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="21"/>
-      <c r="B44" s="5">
-        <v>986691851</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="6">
-        <v>45704.304756944446</v>
-      </c>
-      <c r="E44" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="14">
-        <v>0.12</v>
-      </c>
-      <c r="H44" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B44" s="121">
+        <v>138150122</v>
+      </c>
+      <c r="C44" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="9">
+        <v>45709.465532407405</v>
+      </c>
+      <c r="E44" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="G44" s="118">
+        <v>-1.26</v>
+      </c>
+      <c r="H44" s="50"/>
       <c r="I44" s="21"/>
       <c r="J44" s="21"/>
       <c r="K44" s="21"/>
@@ -4350,27 +4777,27 @@
       <c r="AA44" s="21"/>
       <c r="AB44" s="21"/>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="21"/>
-      <c r="B45" s="8">
-        <v>738944960</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="9">
-        <v>45679.018425925926</v>
-      </c>
-      <c r="E45" s="82" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="46">
-        <v>4.54</v>
-      </c>
-      <c r="H45" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B45" s="133">
+        <v>582941037</v>
+      </c>
+      <c r="C45" s="133" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="134">
+        <v>45895.670243055552</v>
+      </c>
+      <c r="E45" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="139" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="135">
+        <v>1.17</v>
+      </c>
+      <c r="H45" s="50"/>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
       <c r="K45" s="21"/>
@@ -4392,29 +4819,27 @@
       <c r="AA45" s="21"/>
       <c r="AB45" s="21"/>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="21"/>
-      <c r="B46" s="5">
-        <v>355368767</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="6">
-        <v>45682.153043981481</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G46" s="18">
-        <v>-258.39999999999998</v>
-      </c>
-      <c r="H46" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B46" s="136">
+        <v>104729583</v>
+      </c>
+      <c r="C46" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="137">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E46" s="136" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="G46" s="138">
+        <v>-0.32</v>
+      </c>
+      <c r="H46" s="50"/>
       <c r="I46" s="21"/>
       <c r="J46" s="21"/>
       <c r="K46" s="21"/>
@@ -4436,52 +4861,69 @@
       <c r="AA46" s="21"/>
       <c r="AB46" s="21"/>
     </row>
-    <row r="47" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="122">
-        <v>315524141</v>
-      </c>
-      <c r="C47" s="122" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="123">
-        <v>45710.05940972222</v>
-      </c>
-      <c r="E47" s="122" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="124" t="s">
-        <v>40</v>
-      </c>
-      <c r="G47" s="125">
-        <v>-255.6</v>
-      </c>
-      <c r="H47" s="50" t="s">
-        <v>1</v>
-      </c>
+    <row r="47" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="21"/>
+      <c r="B47" s="133">
+        <v>672104958</v>
+      </c>
+      <c r="C47" s="133" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="134">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E47" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" s="139" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="135">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H47" s="50"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="21"/>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="21"/>
+      <c r="X47" s="21"/>
+      <c r="Y47" s="21"/>
+      <c r="Z47" s="21"/>
+      <c r="AA47" s="21"/>
+      <c r="AB47" s="21"/>
     </row>
     <row r="48" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="21"/>
-      <c r="B48" s="112">
-        <v>141056374</v>
-      </c>
-      <c r="C48" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="113">
-        <v>45687.295057870368</v>
-      </c>
-      <c r="E48" s="112" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="G48" s="115">
-        <v>-511.36</v>
-      </c>
-      <c r="H48" s="50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B48" s="136">
+        <v>394857126</v>
+      </c>
+      <c r="C48" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="137">
+        <v>45895.670240844898</v>
+      </c>
+      <c r="E48" s="136" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="G48" s="138">
+        <v>-0.16</v>
+      </c>
+      <c r="H48" s="50"/>
       <c r="I48" s="21"/>
       <c r="J48" s="21"/>
       <c r="K48" s="21"/>
@@ -4503,46 +4945,67 @@
       <c r="AA48" s="21"/>
       <c r="AB48" s="21"/>
     </row>
-    <row r="49" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="107">
-        <v>863763119</v>
-      </c>
-      <c r="C49" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="108">
-        <v>45663.500069444446</v>
-      </c>
-      <c r="E49" s="107" t="s">
-        <v>86</v>
-      </c>
-      <c r="F49" s="110" t="s">
-        <v>27</v>
-      </c>
-      <c r="G49" s="109">
-        <v>6.84</v>
+    <row r="49" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="21"/>
+      <c r="B49" s="5">
+        <v>827364501</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="6">
+        <v>45806.4937884838</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" s="14">
+        <v>22.43</v>
       </c>
       <c r="H49" s="50"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+      <c r="T49" s="21"/>
+      <c r="U49" s="21"/>
+      <c r="V49" s="21"/>
+      <c r="W49" s="21"/>
+      <c r="X49" s="21"/>
+      <c r="Y49" s="21"/>
+      <c r="Z49" s="21"/>
+      <c r="AA49" s="21"/>
+      <c r="AB49" s="21"/>
     </row>
     <row r="50" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="21"/>
-      <c r="B50" s="116">
-        <v>264122037</v>
-      </c>
-      <c r="C50" s="116" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="108">
-        <v>45663.500069444446</v>
-      </c>
-      <c r="E50" s="119" t="s">
-        <v>87</v>
-      </c>
-      <c r="F50" s="117" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="118">
-        <v>-1.03</v>
+      <c r="B50" s="8">
+        <v>210948573</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="9">
+        <v>45806.493810161999</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G50" s="46">
+        <v>28.03</v>
       </c>
       <c r="H50" s="50"/>
       <c r="I50" s="21"/>
@@ -4566,46 +5029,67 @@
       <c r="AA50" s="21"/>
       <c r="AB50" s="21"/>
     </row>
-    <row r="51" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="126">
-        <v>89498937</v>
-      </c>
-      <c r="C51" s="126" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="108">
-        <v>45808.500069444446</v>
-      </c>
-      <c r="E51" s="126" t="s">
-        <v>86</v>
-      </c>
-      <c r="F51" s="127" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" s="109">
-        <v>6.84</v>
+    <row r="51" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="21"/>
+      <c r="B51" s="5">
+        <v>746352910</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="6">
+        <v>45806.493816539398</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="14">
+        <v>44.85</v>
       </c>
       <c r="H51" s="50"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="21"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="21"/>
+      <c r="T51" s="21"/>
+      <c r="U51" s="21"/>
+      <c r="V51" s="21"/>
+      <c r="W51" s="21"/>
+      <c r="X51" s="21"/>
+      <c r="Y51" s="21"/>
+      <c r="Z51" s="21"/>
+      <c r="AA51" s="21"/>
+      <c r="AB51" s="21"/>
     </row>
     <row r="52" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="21"/>
-      <c r="B52" s="119">
-        <v>765529925</v>
-      </c>
-      <c r="C52" s="119" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="108">
-        <v>45808.500069444446</v>
-      </c>
-      <c r="E52" s="119" t="s">
-        <v>87</v>
-      </c>
-      <c r="F52" s="120" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="118">
-        <v>-1.03</v>
+      <c r="B52" s="5">
+        <v>501928374</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="6">
+        <v>45888.497956736101</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="14">
+        <v>4.22</v>
       </c>
       <c r="H52" s="50"/>
       <c r="I52" s="21"/>
@@ -4629,792 +5113,393 @@
       <c r="AA52" s="21"/>
       <c r="AB52" s="21"/>
     </row>
-    <row r="53" spans="1:28" s="21" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="128">
-        <v>488088046</v>
-      </c>
-      <c r="C53" s="126" t="s">
-        <v>31</v>
+    <row r="53" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="21"/>
+      <c r="B53" s="8">
+        <v>883746521</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="D53" s="9">
-        <v>45709.465532407405</v>
-      </c>
-      <c r="E53" s="129" t="s">
-        <v>88</v>
-      </c>
-      <c r="F53" s="130" t="s">
-        <v>89</v>
-      </c>
-      <c r="G53" s="131">
-        <v>4.2</v>
+        <v>45888.497956747698</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G53" s="17">
+        <v>-1.1399999999999999</v>
       </c>
       <c r="H53" s="50"/>
-    </row>
-    <row r="54" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21"/>
-      <c r="B54" s="121">
-        <v>138150122</v>
-      </c>
-      <c r="C54" s="119" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="9">
-        <v>45709.465532407405</v>
-      </c>
-      <c r="E54" s="116" t="s">
-        <v>90</v>
-      </c>
-      <c r="F54" s="117" t="s">
-        <v>89</v>
-      </c>
-      <c r="G54" s="118">
-        <v>-1.26</v>
-      </c>
-      <c r="H54" s="50"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="21"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
-      <c r="Q54" s="21"/>
-      <c r="R54" s="21"/>
-      <c r="S54" s="21"/>
-      <c r="T54" s="21"/>
-      <c r="U54" s="21"/>
-      <c r="V54" s="21"/>
-      <c r="W54" s="21"/>
-      <c r="X54" s="21"/>
-      <c r="Y54" s="21"/>
-      <c r="Z54" s="21"/>
-      <c r="AA54" s="21"/>
-      <c r="AB54" s="21"/>
-    </row>
-    <row r="55" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21"/>
-      <c r="B55" s="133">
-        <v>582941037</v>
-      </c>
-      <c r="C55" s="133" t="s">
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="21"/>
+      <c r="P53" s="21"/>
+      <c r="Q53" s="21"/>
+      <c r="R53" s="21"/>
+      <c r="S53" s="21"/>
+      <c r="T53" s="21"/>
+      <c r="U53" s="21"/>
+      <c r="V53" s="21"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="21"/>
+      <c r="Y53" s="21"/>
+      <c r="Z53" s="21"/>
+      <c r="AA53" s="21"/>
+      <c r="AB53" s="21"/>
+    </row>
+    <row r="54" spans="1:28" s="21" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="5">
+        <v>192837465</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="134">
-        <v>45895.670243055552</v>
-      </c>
-      <c r="E55" s="133" t="s">
-        <v>104</v>
-      </c>
-      <c r="F55" s="139" t="s">
-        <v>105</v>
-      </c>
-      <c r="G55" s="135">
-        <v>1.17</v>
-      </c>
-      <c r="H55" s="50"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="M55" s="21"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="21"/>
-      <c r="S55" s="21"/>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
-      <c r="V55" s="21"/>
-      <c r="W55" s="21"/>
-      <c r="X55" s="21"/>
-      <c r="Y55" s="21"/>
-      <c r="Z55" s="21"/>
-      <c r="AA55" s="21"/>
-      <c r="AB55" s="21"/>
-    </row>
-    <row r="56" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="21"/>
-      <c r="B56" s="136">
-        <v>104729583</v>
-      </c>
-      <c r="C56" s="136" t="s">
+      <c r="D54" s="6">
+        <v>45888.497970567099</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G54" s="14">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B55" s="8">
+        <v>657483920</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D56" s="137">
-        <v>45895.670240844898</v>
-      </c>
-      <c r="E56" s="136" t="s">
-        <v>106</v>
-      </c>
-      <c r="F56" s="140" t="s">
-        <v>105</v>
-      </c>
-      <c r="G56" s="138">
-        <v>-0.32</v>
-      </c>
-      <c r="H56" s="50"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="21"/>
-      <c r="T56" s="21"/>
-      <c r="U56" s="21"/>
-      <c r="V56" s="21"/>
-      <c r="W56" s="21"/>
-      <c r="X56" s="21"/>
-      <c r="Y56" s="21"/>
-      <c r="Z56" s="21"/>
-      <c r="AA56" s="21"/>
-      <c r="AB56" s="21"/>
-    </row>
-    <row r="57" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="21"/>
-      <c r="B57" s="133">
-        <v>672104958</v>
-      </c>
-      <c r="C57" s="133" t="s">
+      <c r="D55" s="9">
+        <v>45888.497970567099</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G55" s="17">
+        <v>-1.71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B56" s="5">
+        <v>435261709</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D57" s="134">
-        <v>45895.670240844898</v>
-      </c>
-      <c r="E57" s="133" t="s">
-        <v>104</v>
-      </c>
-      <c r="F57" s="139" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" s="135">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="H57" s="50"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
-      <c r="S57" s="21"/>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
-      <c r="V57" s="21"/>
-      <c r="W57" s="21"/>
-      <c r="X57" s="21"/>
-      <c r="Y57" s="21"/>
-      <c r="Z57" s="21"/>
-      <c r="AA57" s="21"/>
-      <c r="AB57" s="21"/>
-    </row>
-    <row r="58" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="21"/>
-      <c r="B58" s="136">
-        <v>394857126</v>
-      </c>
-      <c r="C58" s="136" t="s">
+      <c r="D56" s="6">
+        <v>45888.497985914299</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G56" s="14">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B57" s="8">
+        <v>901827364</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D58" s="137">
-        <v>45895.670240844898</v>
-      </c>
-      <c r="E58" s="136" t="s">
-        <v>106</v>
-      </c>
-      <c r="F58" s="140" t="s">
-        <v>105</v>
-      </c>
-      <c r="G58" s="138">
-        <v>-0.16</v>
-      </c>
-      <c r="H58" s="50"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-      <c r="N58" s="21"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="21"/>
-      <c r="Q58" s="21"/>
-      <c r="R58" s="21"/>
-      <c r="S58" s="21"/>
-      <c r="T58" s="21"/>
-      <c r="U58" s="21"/>
-      <c r="V58" s="21"/>
-      <c r="W58" s="21"/>
-      <c r="X58" s="21"/>
-      <c r="Y58" s="21"/>
-      <c r="Z58" s="21"/>
-      <c r="AA58" s="21"/>
-      <c r="AB58" s="21"/>
-    </row>
-    <row r="59" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="21"/>
-      <c r="B59" s="5">
-        <v>827364501</v>
-      </c>
-      <c r="C59" s="5" t="s">
+      <c r="D57" s="9">
+        <v>45888.497986111113</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G57" s="17">
+        <v>-2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B58" s="5">
+        <v>273645109</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="6">
-        <v>45806.4937884838</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G59" s="14">
-        <v>22.43</v>
-      </c>
-      <c r="H59" s="50"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="21"/>
-      <c r="M59" s="21"/>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
-      <c r="P59" s="21"/>
-      <c r="Q59" s="21"/>
-      <c r="R59" s="21"/>
-      <c r="S59" s="21"/>
-      <c r="T59" s="21"/>
-      <c r="U59" s="21"/>
-      <c r="V59" s="21"/>
-      <c r="W59" s="21"/>
-      <c r="X59" s="21"/>
-      <c r="Y59" s="21"/>
-      <c r="Z59" s="21"/>
-      <c r="AA59" s="21"/>
-      <c r="AB59" s="21"/>
-    </row>
-    <row r="60" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="21"/>
-      <c r="B60" s="8">
-        <v>210948573</v>
-      </c>
-      <c r="C60" s="8" t="s">
+      <c r="D58" s="6">
+        <v>45888.497991967597</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G58" s="14">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B59" s="8">
+        <v>510293847</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="9">
+        <v>45888.497991979202</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G59" s="17">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B60" s="5">
+        <v>647583920</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D60" s="9">
-        <v>45806.493810161999</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G60" s="46">
-        <v>28.03</v>
-      </c>
-      <c r="H60" s="50"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
-      <c r="N60" s="21"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="21"/>
-      <c r="Q60" s="21"/>
-      <c r="R60" s="21"/>
-      <c r="S60" s="21"/>
-      <c r="T60" s="21"/>
-      <c r="U60" s="21"/>
-      <c r="V60" s="21"/>
-      <c r="W60" s="21"/>
-      <c r="X60" s="21"/>
-      <c r="Y60" s="21"/>
-      <c r="Z60" s="21"/>
-      <c r="AA60" s="21"/>
-      <c r="AB60" s="21"/>
-    </row>
-    <row r="61" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="21"/>
-      <c r="B61" s="5">
-        <v>746352910</v>
-      </c>
-      <c r="C61" s="5" t="s">
+      <c r="D60" s="6">
+        <v>45888.498006701397</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G60" s="14">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B61" s="8">
+        <v>384756291</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="9">
+        <v>45888.498006713002</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G61" s="17">
+        <v>-1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B62" s="8">
+        <v>726354810</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D61" s="6">
-        <v>45806.493816539398</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G61" s="14">
-        <v>44.85</v>
-      </c>
-      <c r="H61" s="50"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-      <c r="N61" s="21"/>
-      <c r="O61" s="21"/>
-      <c r="P61" s="21"/>
-      <c r="Q61" s="21"/>
-      <c r="R61" s="21"/>
-      <c r="S61" s="21"/>
-      <c r="T61" s="21"/>
-      <c r="U61" s="21"/>
-      <c r="V61" s="21"/>
-      <c r="W61" s="21"/>
-      <c r="X61" s="21"/>
-      <c r="Y61" s="21"/>
-      <c r="Z61" s="21"/>
-      <c r="AA61" s="21"/>
-      <c r="AB61" s="21"/>
-    </row>
-    <row r="62" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="21"/>
-      <c r="B62" s="5">
-        <v>501928374</v>
-      </c>
-      <c r="C62" s="5" t="s">
+      <c r="D62" s="9">
+        <v>45833.328140034697</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" s="46">
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B63" s="5">
+        <v>819203746</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="6">
+        <v>45833.328140034697</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="18">
+        <v>-8.2799999999999994</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B64" s="8">
+        <v>152637489</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D62" s="6">
-        <v>45888.497956736101</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G62" s="14">
-        <v>4.22</v>
-      </c>
-      <c r="H62" s="50"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="21"/>
-      <c r="O62" s="21"/>
-      <c r="P62" s="21"/>
-      <c r="Q62" s="21"/>
-      <c r="R62" s="21"/>
-      <c r="S62" s="21"/>
-      <c r="T62" s="21"/>
-      <c r="U62" s="21"/>
-      <c r="V62" s="21"/>
-      <c r="W62" s="21"/>
-      <c r="X62" s="21"/>
-      <c r="Y62" s="21"/>
-      <c r="Z62" s="21"/>
-      <c r="AA62" s="21"/>
-      <c r="AB62" s="21"/>
-    </row>
-    <row r="63" spans="1:28" s="111" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="21"/>
-      <c r="B63" s="8">
-        <v>883746521</v>
-      </c>
-      <c r="C63" s="8" t="s">
+      <c r="D64" s="9">
+        <v>45833.3282088079</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G64" s="46">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="5">
+        <v>948576102</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="9">
-        <v>45888.497956747698</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G63" s="17">
-        <v>-1.1399999999999999</v>
-      </c>
-      <c r="H63" s="50"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
-      <c r="N63" s="21"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="21"/>
-      <c r="R63" s="21"/>
-      <c r="S63" s="21"/>
-      <c r="T63" s="21"/>
-      <c r="U63" s="21"/>
-      <c r="V63" s="21"/>
-      <c r="W63" s="21"/>
-      <c r="X63" s="21"/>
-      <c r="Y63" s="21"/>
-      <c r="Z63" s="21"/>
-      <c r="AA63" s="21"/>
-      <c r="AB63" s="21"/>
-    </row>
-    <row r="64" spans="1:28" s="21" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="5">
-        <v>192837465</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="D65" s="6">
+        <v>45833.3282088079</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" s="18">
+        <v>-4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="8">
+        <v>203948576</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D64" s="6">
-        <v>45888.497970567099</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G64" s="14">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="8">
-        <v>657483920</v>
-      </c>
-      <c r="C65" s="8" t="s">
+      <c r="D66" s="9">
+        <v>45833.328220092597</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="46">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="5">
+        <v>475869201</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D65" s="9">
-        <v>45888.497970567099</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G65" s="17">
-        <v>-1.71</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="5">
-        <v>435261709</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="D67" s="6">
+        <v>45833.328220092597</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="18">
+        <v>-5.18</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="8">
+        <v>364758291</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="6">
-        <v>45888.497985914299</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G66" s="14">
-        <v>8.44</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="8">
-        <v>901827364</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D67" s="9">
-        <v>45888.497986111113</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G67" s="17">
-        <v>-2.2799999999999998</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="5">
-        <v>273645109</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D68" s="6">
-        <v>45888.497991967597</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G68" s="14">
-        <v>4.22</v>
+      <c r="D68" s="9">
+        <v>45944.3284375</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G68" s="46">
+        <v>38.15</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B69" s="8">
-        <v>510293847</v>
-      </c>
-      <c r="C69" s="8" t="s">
+        <v>657483926</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D69" s="9">
-        <v>45888.497991979202</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G69" s="17">
-        <v>-1.1399999999999999</v>
+        <v>45944.3284375</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G69" s="18">
+        <v>-7.25</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B70" s="5">
-        <v>647583920</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D70" s="6">
-        <v>45888.498006701397</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G70" s="14">
-        <v>4.22</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B71" s="8">
-        <v>384756291</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D71" s="9">
-        <v>45888.498006713002</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G71" s="17">
-        <v>-1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B72" s="8">
-        <v>726354810</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D72" s="9">
-        <v>45833.328140034697</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G72" s="46">
-        <v>43.6</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B73" s="5">
-        <v>819203746</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D73" s="6">
-        <v>45833.328140034697</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G73" s="18">
-        <v>-8.2799999999999994</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B74" s="8">
-        <v>152637489</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D74" s="9">
-        <v>45833.3282088079</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G74" s="46">
-        <v>21.8</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B75" s="5">
-        <v>948576102</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D75" s="6">
-        <v>45833.3282088079</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G75" s="18">
-        <v>-4.1399999999999997</v>
+      <c r="B70" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="51"/>
+      <c r="G70" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="H70" s="51" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B76" s="8">
-        <v>203948576</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" s="9">
-        <v>45833.328220092597</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G76" s="46">
-        <v>27.25</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B77" s="5">
-        <v>475869201</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D77" s="6">
-        <v>45833.328220092597</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G77" s="18">
-        <v>-5.18</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B78" s="8">
-        <v>364758291</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="9">
-        <v>45944.3284375</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F78" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G78" s="46">
-        <v>38.15</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B79" s="8">
-        <v>657483926</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D79" s="9">
-        <v>45944.3284375</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G79" s="18">
-        <v>-7.25</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B80" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="F80" s="51"/>
-      <c r="G80" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="H80" s="51" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B86" s="32"/>
-      <c r="C86" s="32"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="33"/>
-      <c r="H86" s="51"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5476,7 +5561,7 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:38" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="141" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="142"/>
@@ -5519,7 +5604,7 @@
       <c r="V4" s="142"/>
     </row>
     <row r="5" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="143" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="142"/>
@@ -5560,14 +5645,14 @@
       <c r="R5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="151" t="s">
+      <c r="S5" s="144" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="142"/>
       <c r="U5" s="142"/>
     </row>
     <row r="6" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="152" t="s">
+      <c r="B6" s="145" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="142"/>
@@ -5604,18 +5689,18 @@
       <c r="R6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="151" t="s">
+      <c r="S6" s="144" t="s">
         <v>1</v>
       </c>
       <c r="T6" s="142"/>
       <c r="U6" s="142"/>
     </row>
     <row r="7" spans="1:38" s="21" customFormat="1" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="163" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="142"/>
-      <c r="D7" s="163" t="s">
+      <c r="D7" s="164" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="142"/>
@@ -5658,7 +5743,7 @@
       <c r="R7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="163" t="s">
+      <c r="S7" s="164" t="s">
         <v>1</v>
       </c>
       <c r="T7" s="142"/>
@@ -5666,14 +5751,14 @@
     </row>
     <row r="8" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
-      <c r="B8" s="145">
+      <c r="B8" s="149">
         <v>442606945</v>
       </c>
-      <c r="C8" s="146"/>
-      <c r="D8" s="164" t="s">
+      <c r="C8" s="150"/>
+      <c r="D8" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="146"/>
+      <c r="E8" s="150"/>
       <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
@@ -5714,11 +5799,11 @@
       <c r="R8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="161" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="158"/>
-      <c r="U8" s="158"/>
+      <c r="S8" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="157"/>
+      <c r="U8" s="157"/>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
       <c r="X8" s="21"/>
@@ -5739,14 +5824,14 @@
     </row>
     <row r="9" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
-      <c r="B9" s="155">
+      <c r="B9" s="158">
         <v>654595998</v>
       </c>
-      <c r="C9" s="146"/>
-      <c r="D9" s="156" t="s">
+      <c r="C9" s="150"/>
+      <c r="D9" s="159" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="156"/>
+      <c r="E9" s="159"/>
       <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
@@ -5787,11 +5872,11 @@
       <c r="R9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="157" t="s">
-        <v>1</v>
-      </c>
-      <c r="T9" s="158"/>
-      <c r="U9" s="158"/>
+      <c r="S9" s="160" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="157"/>
+      <c r="U9" s="157"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
@@ -5812,14 +5897,14 @@
     </row>
     <row r="10" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
-      <c r="B10" s="145">
+      <c r="B10" s="149">
         <v>620339720</v>
       </c>
-      <c r="C10" s="146"/>
-      <c r="D10" s="159" t="s">
+      <c r="C10" s="150"/>
+      <c r="D10" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="160"/>
+      <c r="E10" s="162"/>
       <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
@@ -5860,11 +5945,11 @@
       <c r="R10" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="161" t="s">
-        <v>1</v>
-      </c>
-      <c r="T10" s="158"/>
-      <c r="U10" s="158"/>
+      <c r="S10" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
@@ -5884,11 +5969,11 @@
       <c r="AL10" s="21"/>
     </row>
     <row r="11" spans="1:38" s="21" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="146" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="142"/>
-      <c r="D11" s="141" t="s">
+      <c r="D11" s="146" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="142"/>
@@ -5930,7 +6015,7 @@
       <c r="R11" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="141" t="s">
+      <c r="S11" s="146" t="s">
         <v>1</v>
       </c>
       <c r="T11" s="142"/>
@@ -5941,11 +6026,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="S5:U5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="S11:U11"/>
@@ -5962,6 +6042,11 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6015,7 +6100,7 @@
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:29" s="21" customFormat="1" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="141" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="142"/>
@@ -6031,7 +6116,7 @@
       <c r="I4" s="142"/>
     </row>
     <row r="5" spans="1:29" s="21" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="143" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="142"/>

</xml_diff>